<commit_message>
small amendment to HCC summary xlsx
</commit_message>
<xml_diff>
--- a/hccPublicData/summary.xlsx
+++ b/hccPublicData/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/ba1e12_soton_ac_uk/Documents/R/github/HCC_dataExpertGroup/publicData/hccPublicData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BDCB0C0-7EA7-0D49-81ED-46DE4547C928}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3BDCB0C0-7EA7-0D49-81ED-46DE4547C928}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F15081B9-C46A-2A42-B322-DDD0AB0122B9}"/>
   <bookViews>
-    <workbookView xWindow="16000" yWindow="4240" windowWidth="21980" windowHeight="14460" activeTab="2" xr2:uid="{1159E10A-BDF6-5940-85F3-1CD8C5AA97CE}"/>
+    <workbookView xWindow="10540" yWindow="4900" windowWidth="21980" windowHeight="14460" activeTab="2" xr2:uid="{1159E10A-BDF6-5940-85F3-1CD8C5AA97CE}"/>
   </bookViews>
   <sheets>
     <sheet name="HCC estimates" sheetId="1" r:id="rId1"/>
@@ -923,6 +923,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>